<commit_message>
Gets the ss of no error pages.
</commit_message>
<xml_diff>
--- a/Nodes.xlsx
+++ b/Nodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YPN-1135\Desktop\NodeBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A501EA7-3B7A-4F69-A15A-38D60D3125AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63B1972-B828-4A6E-A83B-362F40C1F147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3450" yWindow="3450" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>NODES</t>
   </si>
   <si>
     <t>F2 Nodes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">201671, 276616, 276617 </t>
   </si>
 </sst>
 </file>
@@ -95,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -148,11 +148,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -164,6 +179,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -447,15 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,65 +481,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A2" s="6">
+        <v>146568</v>
       </c>
       <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A3" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A3" s="6">
+        <v>202047</v>
+      </c>
       <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A4" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A4" s="6">
+        <v>215069</v>
+      </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A5" s="3">
+        <v>279290</v>
+      </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A6" s="3"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A7" s="3"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A8" s="3"/>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A9" s="3"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A10" s="2"/>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A10" s="3"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A11" s="3"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A12" s="2"/>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A12" s="3"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A13" s="5"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A14" s="5"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A15" s="2"/>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A15" s="5"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1" thickBot="1">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" thickBot="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
     </row>

</xml_diff>